<commit_message>
Update export mutasi saldo
</commit_message>
<xml_diff>
--- a/storage/app/report-template/finance.xlsx
+++ b/storage/app/report-template/finance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Tanggal</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">Keterangan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User</t>
   </si>
   <si>
     <t xml:space="preserve">Kredit</t>
@@ -152,19 +155,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9109311740891"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.7125506072874"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="2" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="2" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -177,7 +181,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -185,6 +189,9 @@
       </c>
       <c r="F1" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>